<commit_message>
Refactro usdm tag handling, preprocess more
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/encounter_1.xlsx
+++ b/tests/integration_test_files/encounter_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E3B3D8-13D2-DC44-921D-D36CC00E46FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048780BF-7CAD-FB45-B258-90FFB174E2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="9" activeTab="19" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="11" activeTab="21" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1885,15 +1885,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>&lt;usdm:section name="M11-title-page"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;usdm:section name="M11-inclusion"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;usdm:section name="M11-exclusion"&gt;</t>
-  </si>
-  <si>
     <t>Exclusion</t>
   </si>
   <si>
@@ -1924,9 +1915,6 @@
     <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia over the age of [min_age]</t>
   </si>
   <si>
-    <t>&lt;usdm:section name="M11-objective-endpoints"&gt;</t>
-  </si>
-  <si>
     <t>Berber_Dict</t>
   </si>
   <si>
@@ -2327,6 +2315,18 @@
   </si>
   <si>
     <t>In Person, TELEPHONE CALL</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="section" name="title_page" template="m11"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="section" name="objective_endpoints" template="m11"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="section" name="inclusion" template="m11"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="section" name="exclusion" template="m11"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2550,10 +2550,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2580,9 +2580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2620,7 +2620,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2726,7 +2726,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2868,7 +2868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B7" t="s">
         <v>579</v>
@@ -3660,24 +3660,24 @@
         <v>194</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>598</v>
@@ -3688,16 +3688,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>598</v>
@@ -3708,16 +3708,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>752</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" t="s">
@@ -3838,7 +3838,7 @@
         <v>460</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>44</v>
@@ -3849,13 +3849,13 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C2" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -3866,10 +3866,10 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>130</v>
@@ -3929,49 +3929,49 @@
         <v>44</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>669</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>670</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>671</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>666</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>667</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>668</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>669</v>
-      </c>
-      <c r="J1" s="18" t="s">
+      <c r="P1" s="18" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>674</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>675</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>670</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>671</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>672</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>677</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>678</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -3979,58 +3979,58 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
+        <v>676</v>
+      </c>
+      <c r="C2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D2" t="s">
+        <v>678</v>
+      </c>
+      <c r="E2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>693</v>
+      </c>
+      <c r="G2" t="s">
+        <v>679</v>
+      </c>
+      <c r="H2" t="s">
+        <v>682</v>
+      </c>
+      <c r="I2" t="s">
         <v>680</v>
       </c>
-      <c r="C2" t="s">
-        <v>681</v>
-      </c>
-      <c r="D2" t="s">
-        <v>682</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
+        <v>683</v>
+      </c>
+      <c r="K2" t="s">
+        <v>684</v>
+      </c>
+      <c r="L2" t="s">
         <v>685</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>697</v>
-      </c>
-      <c r="G2" t="s">
-        <v>683</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
+        <v>691</v>
+      </c>
+      <c r="N2" t="s">
         <v>686</v>
       </c>
-      <c r="I2" t="s">
-        <v>684</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
+        <v>692</v>
+      </c>
+      <c r="P2" t="s">
         <v>687</v>
-      </c>
-      <c r="K2" t="s">
-        <v>688</v>
-      </c>
-      <c r="L2" t="s">
-        <v>689</v>
-      </c>
-      <c r="M2" t="s">
-        <v>695</v>
-      </c>
-      <c r="N2" t="s">
-        <v>690</v>
-      </c>
-      <c r="O2" t="s">
-        <v>696</v>
-      </c>
-      <c r="P2" t="s">
-        <v>691</v>
       </c>
       <c r="Q2" t="s">
         <v>130</v>
       </c>
       <c r="R2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -4038,58 +4038,58 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
+        <v>694</v>
+      </c>
+      <c r="C3" t="s">
+        <v>695</v>
+      </c>
+      <c r="D3" t="s">
+        <v>678</v>
+      </c>
+      <c r="E3" t="s">
+        <v>696</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>693</v>
+      </c>
+      <c r="G3" t="s">
+        <v>679</v>
+      </c>
+      <c r="H3" t="s">
+        <v>697</v>
+      </c>
+      <c r="I3" t="s">
+        <v>680</v>
+      </c>
+      <c r="J3" t="s">
         <v>698</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" t="s">
         <v>699</v>
       </c>
-      <c r="D3" t="s">
-        <v>682</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="L3" t="s">
         <v>700</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>697</v>
-      </c>
-      <c r="G3" t="s">
-        <v>683</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
+        <v>691</v>
+      </c>
+      <c r="N3" t="s">
+        <v>686</v>
+      </c>
+      <c r="O3" t="s">
+        <v>692</v>
+      </c>
+      <c r="P3" t="s">
         <v>701</v>
-      </c>
-      <c r="I3" t="s">
-        <v>684</v>
-      </c>
-      <c r="J3" t="s">
-        <v>702</v>
-      </c>
-      <c r="K3" t="s">
-        <v>703</v>
-      </c>
-      <c r="L3" t="s">
-        <v>704</v>
-      </c>
-      <c r="M3" t="s">
-        <v>695</v>
-      </c>
-      <c r="N3" t="s">
-        <v>690</v>
-      </c>
-      <c r="O3" t="s">
-        <v>696</v>
-      </c>
-      <c r="P3" t="s">
-        <v>705</v>
       </c>
       <c r="Q3" t="s">
         <v>130</v>
       </c>
       <c r="R3" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -4119,7 +4119,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>389</v>
@@ -4131,24 +4131,24 @@
         <v>460</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B2" t="s">
         <v>503</v>
@@ -4168,13 +4168,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B3" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="G3" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>130</v>
@@ -4182,13 +4182,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B4" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="G4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>130</v>
@@ -4240,7 +4240,7 @@
         <v>51</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>514</v>
@@ -4261,7 +4261,7 @@
         <v>53</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -4303,13 +4303,13 @@
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>71</v>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -4974,7 +4974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -5134,7 +5134,7 @@
         <v>139</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>578</v>
@@ -5160,7 +5160,7 @@
         <v>142</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -5298,8 +5298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5333,7 +5333,7 @@
         <v>606</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>608</v>
+        <v>752</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5409,7 +5409,7 @@
         <v>458</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>621</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5527,7 +5527,7 @@
         <v>215</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>609</v>
+        <v>754</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5539,7 +5539,7 @@
         <v>216</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>610</v>
+        <v>755</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6603,94 +6603,94 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
+        <v>629</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>633</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B10" s="39"/>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -6792,53 +6792,53 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B4" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C4" t="s">
+        <v>651</v>
+      </c>
+      <c r="D4" t="s">
+        <v>650</v>
+      </c>
+      <c r="E4" t="s">
         <v>655</v>
-      </c>
-      <c r="D4" t="s">
-        <v>654</v>
-      </c>
-      <c r="E4" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C5" t="s">
+        <v>652</v>
+      </c>
+      <c r="D5" t="s">
         <v>650</v>
       </c>
-      <c r="B5" t="s">
-        <v>653</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>656</v>
-      </c>
-      <c r="D5" t="s">
-        <v>654</v>
-      </c>
-      <c r="E5" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B6" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C6" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D6" t="s">
         <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -6887,34 +6887,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -6951,10 +6951,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -6962,10 +6962,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
@@ -6973,10 +6973,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
@@ -7067,11 +7067,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B8:E8"/>
@@ -7080,6 +7075,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7116,30 +7116,30 @@
         <v>42</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>493</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>728</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>113</v>
@@ -7154,33 +7154,33 @@
         <v>604</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F3"/>
       <c r="G3" s="3" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>113</v>
@@ -7195,13 +7195,13 @@
         <v>605</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -7470,39 +7470,39 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>506</v>
       </c>
       <c r="C4" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D4" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F4" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>510</v>
       </c>
       <c r="C5" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D5" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="F5" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="G5" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -7571,7 +7571,7 @@
         <v>503</v>
       </c>
       <c r="G2" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -7585,18 +7585,18 @@
         <v>503</v>
       </c>
       <c r="G3" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B4" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C4" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D4" t="s">
         <v>501</v>
@@ -7608,21 +7608,21 @@
         <v>503</v>
       </c>
       <c r="G4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B5" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C5" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D5" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E5" t="s">
         <v>548</v>

</xml_diff>